<commit_message>
Verify membership in orange website
</commit_message>
<xml_diff>
--- a/test_data/orange_data.xlsx
+++ b/test_data/orange_data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmergencyContacts" sheetId="1" r:id="rId1"/>
+    <sheet name="AddMemberships" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>${username}</t>
   </si>
@@ -54,6 +55,27 @@
   </si>
   <si>
     <t>${contact_name}</t>
+  </si>
+  <si>
+    <t>${paid_by}</t>
+  </si>
+  <si>
+    <t>${amount}</t>
+  </si>
+  <si>
+    <t>${membership}</t>
+  </si>
+  <si>
+    <t>${coin}</t>
+  </si>
+  <si>
+    <t>CIMA</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Indian Rupee</t>
   </si>
 </sst>
 </file>
@@ -373,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -441,4 +463,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>